<commit_message>
Update HTBO with number of levels
</commit_message>
<xml_diff>
--- a/static/HTBO.xlsx
+++ b/static/HTBO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kobi/Documents/Research/phd_code/other/htbo_app/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA9B7A86-456A-0A4C-9BE4-A201A5348EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F157B3E-792A-A549-AEB3-F212A8D40E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{C7B5DD84-15C8-B24D-A840-1FA0510D206E}"/>
+    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{C7B5DD84-15C8-B24D-A840-1FA0510D206E}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="10" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Solvents" sheetId="1" r:id="rId3"/>
     <sheet name="Bases" sheetId="2" r:id="rId4"/>
     <sheet name="Catalyst" sheetId="3" r:id="rId5"/>
-    <sheet name="Options" sheetId="4" state="hidden" r:id="rId6"/>
+    <sheet name="Options" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Solvents!$A$1:$E$273</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="325">
   <si>
     <t>Name</t>
   </si>
@@ -863,12 +863,6 @@
     <t>Triacetin [1,2,3-triacetoxypropane]</t>
   </si>
   <si>
-    <t>Approved</t>
-  </si>
-  <si>
-    <t>Not Approved</t>
-  </si>
-  <si>
     <t>Adjusted ranking</t>
   </si>
   <si>
@@ -887,9 +881,6 @@
     <t>CAS number</t>
   </si>
   <si>
-    <t>Approval</t>
-  </si>
-  <si>
     <t>Potassium carbonate</t>
   </si>
   <si>
@@ -908,69 +899,15 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Reactant 1 Concentration</t>
-  </si>
-  <si>
     <t>Continuous</t>
   </si>
   <si>
-    <t>Reactant 2 Equivalents</t>
-  </si>
-  <si>
-    <t>Catalyst Loading</t>
-  </si>
-  <si>
-    <t>Base Loading</t>
-  </si>
-  <si>
-    <t>Solvent 1</t>
-  </si>
-  <si>
-    <t>Solvent 1 Fraction</t>
-  </si>
-  <si>
-    <t>Solvent 2</t>
-  </si>
-  <si>
-    <t>Solvent 2 Fraction</t>
-  </si>
-  <si>
-    <t>Complexation Additive</t>
-  </si>
-  <si>
-    <t>Complexation Temperature</t>
-  </si>
-  <si>
-    <t>Reaction Temperature</t>
-  </si>
-  <si>
     <t>Categorical</t>
   </si>
   <si>
-    <t>Catalyst</t>
-  </si>
-  <si>
-    <t>Base</t>
-  </si>
-  <si>
-    <t>Irradiation Wavelength</t>
-  </si>
-  <si>
-    <t>Complexation Time</t>
-  </si>
-  <si>
-    <t>Reaction Time</t>
-  </si>
-  <si>
     <t>C(=O)([O-])[O-].[K+].[K+]</t>
   </si>
   <si>
-    <t>Yield</t>
-  </si>
-  <si>
-    <t>Selectivity</t>
-  </si>
-  <si>
     <t>Maximize</t>
   </si>
   <si>
@@ -1065,13 +1002,28 @@
   </si>
   <si>
     <t>Optimize</t>
+  </si>
+  <si>
+    <t>Exclude</t>
+  </si>
+  <si>
+    <t>Include</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Reaction Scheme</t>
+  </si>
+  <si>
+    <t># Levels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1094,6 +1046,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -1109,18 +1068,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1135,21 +1088,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1171,23 +1115,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1241,12 +1188,62 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEDE242D-7C8F-2496-1EE3-C5163AA61CBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4076700" y="1066800"/>
+          <a:ext cx="4864100" cy="1612900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78F4AB6B-B01A-DE44-9BB5-9DF01F848148}" name="Table32" displayName="Table32" ref="D4:K22" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="D4:K22" xr:uid="{78F4AB6B-B01A-DE44-9BB5-9DF01F848148}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78F4AB6B-B01A-DE44-9BB5-9DF01F848148}" name="Table32" displayName="Table32" ref="D17:L35" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="D17:L35" xr:uid="{78F4AB6B-B01A-DE44-9BB5-9DF01F848148}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{69A178D2-F201-2246-9870-9B71BC47B817}" name="Name"/>
     <tableColumn id="2" xr3:uid="{9FDE7D9D-63AF-6942-8B05-610F70754415}" name="Type"/>
+    <tableColumn id="10" xr3:uid="{CE1B4B21-0560-2346-9D00-E9A60D254CD4}" name="# Levels"/>
     <tableColumn id="8" xr3:uid="{6356CFEC-090B-AD47-8836-BB0FF79D71DB}" name="Optimize"/>
     <tableColumn id="9" xr3:uid="{CF2C97C9-E6A8-CB4E-9C4F-50CCB04E389C}" name="Categorical Levels"/>
     <tableColumn id="3" xr3:uid="{71C1FA1B-B214-4946-92F6-A5E37087362B}" name="Units"/>
@@ -1555,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD37251-C0AB-6A41-A851-086D682EF19C}">
-  <dimension ref="B1:K22"/>
+  <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1566,33 +1563,33 @@
     <col min="1" max="1" width="4.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B1" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="3" spans="2:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="B1" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>338</v>
-      </c>
+        <v>323</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
@@ -1600,247 +1597,429 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="16" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="7"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="7"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="7"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="E17" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="B1:K1"/>
+  <mergeCells count="3">
+    <mergeCell ref="D16:L16"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B3:L14"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Select categorical levels" prompt="Choose a categorical sheet with levels to use for this variable." sqref="G5:G22" xr:uid="{3639F545-7D47-2B48-96BC-F69FA641A739}">
-      <formula1>$B$4:$B$11</formula1>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Select categorical levels" prompt="Choose a categorical sheet with levels to use for this variable." sqref="H18:H35" xr:uid="{3639F545-7D47-2B48-96BC-F69FA641A739}">
+      <formula1>$B$17:$B$24</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select categorical sheet" prompt="Choose a categorical sheet with levels to use for this variable." sqref="G4" xr:uid="{64E5C515-5F83-4A4A-A337-85E8CDEA2B94}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optimize" prompt="Select if this variable that should maximized or minimized. If not, leave blank." sqref="F4" xr:uid="{7DD73263-1F88-4745-82C0-359895234AB1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Units" prompt="For continuous variables, record the units!" sqref="H4" xr:uid="{456B3843-60A3-454D-93D6-9058576C5C23}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Lower limit" prompt="This is the lower limit on continous variables. Leave blank for categorical variables." sqref="I4" xr:uid="{8627930E-DD22-DD48-824B-6EE6624C3372}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Upper limit" prompt="This is the upper limit on continous variables. Leave blank for categorical variables." sqref="J4" xr:uid="{0443F521-5F07-C642-8438-B5952D5C0EEE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select categorical sheet" prompt="Choose a categorical sheet with levels to use for this variable." sqref="H17" xr:uid="{64E5C515-5F83-4A4A-A337-85E8CDEA2B94}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optimize" prompt="Select if this variable that should maximized or minimized. If not, leave blank." sqref="G17" xr:uid="{7DD73263-1F88-4745-82C0-359895234AB1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Units" prompt="For continuous variables, record the units!" sqref="I17" xr:uid="{456B3843-60A3-454D-93D6-9058576C5C23}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Lower limit" prompt="This is the lower limit on continous variables. Leave blank for categorical variables." sqref="J17" xr:uid="{8627930E-DD22-DD48-824B-6EE6624C3372}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Upper limit" prompt="This is the upper limit on continous variables. Leave blank for categorical variables." sqref="K17" xr:uid="{0443F521-5F07-C642-8438-B5952D5C0EEE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Number of levels" prompt="The number of levels of this variable to select in each batch." sqref="F17" xr:uid="{4D911236-9B9B-E840-9CD7-A6EFDB2A0FB7}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1849,13 +2028,13 @@
           <x14:formula1>
             <xm:f>Options!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>F5:F22</xm:sqref>
+          <xm:sqref>G18:G35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBD807DE-ACF9-AB46-AD57-FC74F23D025B}">
           <x14:formula1>
             <xm:f>Options!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>E5:E22</xm:sqref>
+          <xm:sqref>E18:E35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1865,10 +2044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1198AFB5-CB38-9A44-9E53-A36E0E515F6F}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1888,64 +2067,7 @@
     <col min="15" max="15" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1954,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6DB1A3-35C8-5847-B5DD-3DD6FA544F70}">
   <dimension ref="A1:E407"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1970,16 +2092,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>281</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1987,10 +2109,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E2" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1998,10 +2120,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E3" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2009,10 +2131,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E4" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2020,10 +2142,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E5" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2031,10 +2153,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E6" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2042,10 +2164,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E7" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2053,10 +2175,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E8" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2064,10 +2186,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E9" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2075,10 +2197,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E10" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2086,10 +2208,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E11" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2097,10 +2219,10 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E12" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2108,10 +2230,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E13" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2119,10 +2241,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E14" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -2130,10 +2252,10 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E15" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2141,10 +2263,10 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E16" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2152,10 +2274,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E17" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2163,10 +2285,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E18" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2174,10 +2296,10 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E19" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2185,10 +2307,10 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E20" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2196,10 +2318,10 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E21" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2207,10 +2329,10 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E22" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2218,10 +2340,10 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E23" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2229,10 +2351,10 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E24" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2240,10 +2362,10 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E25" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2251,10 +2373,10 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E26" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -2262,10 +2384,10 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E27" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -2273,10 +2395,10 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E28" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2284,10 +2406,10 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E29" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -2295,10 +2417,10 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E30" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -2306,10 +2428,10 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E31" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -2317,10 +2439,10 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E32" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -2328,10 +2450,10 @@
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E33" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2339,10 +2461,10 @@
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E34" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -2350,10 +2472,10 @@
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E35" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -2361,10 +2483,10 @@
         <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E36" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -2372,10 +2494,10 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E37" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2383,10 +2505,10 @@
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E38" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -2394,10 +2516,10 @@
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E39" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -2405,10 +2527,10 @@
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E40" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2416,10 +2538,10 @@
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E41" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2427,10 +2549,10 @@
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E42" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -2438,10 +2560,10 @@
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E43" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -2449,10 +2571,10 @@
         <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E44" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -2460,10 +2582,10 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E45" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -2471,10 +2593,10 @@
         <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E46" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -2482,10 +2604,10 @@
         <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E47" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -2493,10 +2615,10 @@
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E48" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -2504,10 +2626,10 @@
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E49" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -2515,10 +2637,10 @@
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E50" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -2526,10 +2648,10 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E51" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -2537,10 +2659,10 @@
         <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E52" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -2548,10 +2670,10 @@
         <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E53" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -2559,10 +2681,10 @@
         <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E54" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -2570,10 +2692,10 @@
         <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E55" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -2581,10 +2703,10 @@
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E56" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2592,10 +2714,10 @@
         <v>56</v>
       </c>
       <c r="D57" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E57" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2603,10 +2725,10 @@
         <v>57</v>
       </c>
       <c r="D58" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E58" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2614,10 +2736,10 @@
         <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E59" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2625,10 +2747,10 @@
         <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E60" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2636,10 +2758,10 @@
         <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E61" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2647,10 +2769,10 @@
         <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E62" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2658,10 +2780,10 @@
         <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E63" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2669,10 +2791,10 @@
         <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E64" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -2680,10 +2802,10 @@
         <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E65" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2691,10 +2813,10 @@
         <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E66" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2702,10 +2824,10 @@
         <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E67" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -2713,10 +2835,10 @@
         <v>67</v>
       </c>
       <c r="D68" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E68" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2724,10 +2846,10 @@
         <v>68</v>
       </c>
       <c r="D69" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E69" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -2735,10 +2857,10 @@
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E70" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -2746,10 +2868,10 @@
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E71" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -2757,10 +2879,10 @@
         <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E72" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -2768,10 +2890,10 @@
         <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E73" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2779,10 +2901,10 @@
         <v>73</v>
       </c>
       <c r="D74" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E74" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -2790,10 +2912,10 @@
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E75" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -2801,10 +2923,10 @@
         <v>75</v>
       </c>
       <c r="D76" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E76" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2812,10 +2934,10 @@
         <v>76</v>
       </c>
       <c r="D77" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E77" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2823,10 +2945,10 @@
         <v>77</v>
       </c>
       <c r="D78" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E78" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2834,10 +2956,10 @@
         <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E79" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2845,10 +2967,10 @@
         <v>79</v>
       </c>
       <c r="D80" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E80" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2856,10 +2978,10 @@
         <v>80</v>
       </c>
       <c r="D81" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E81" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2867,10 +2989,10 @@
         <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E82" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2878,10 +3000,10 @@
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E83" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2889,10 +3011,10 @@
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E84" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2900,10 +3022,10 @@
         <v>84</v>
       </c>
       <c r="D85" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E85" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2911,10 +3033,10 @@
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E86" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2922,10 +3044,10 @@
         <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E87" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2933,10 +3055,10 @@
         <v>87</v>
       </c>
       <c r="D88" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E88" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2944,10 +3066,10 @@
         <v>88</v>
       </c>
       <c r="D89" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E89" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2955,10 +3077,10 @@
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E90" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -2966,10 +3088,10 @@
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E91" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2977,10 +3099,10 @@
         <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E92" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2988,10 +3110,10 @@
         <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E93" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2999,10 +3121,10 @@
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E94" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -3010,10 +3132,10 @@
         <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E95" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -3021,10 +3143,10 @@
         <v>95</v>
       </c>
       <c r="D96" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E96" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -3032,10 +3154,10 @@
         <v>96</v>
       </c>
       <c r="D97" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E97" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -3043,10 +3165,10 @@
         <v>97</v>
       </c>
       <c r="D98" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E98" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -3054,10 +3176,10 @@
         <v>98</v>
       </c>
       <c r="D99" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E99" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -3065,10 +3187,10 @@
         <v>99</v>
       </c>
       <c r="D100" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E100" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -3076,10 +3198,10 @@
         <v>100</v>
       </c>
       <c r="D101" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E101" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -3087,10 +3209,10 @@
         <v>101</v>
       </c>
       <c r="D102" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E102" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -3098,10 +3220,10 @@
         <v>102</v>
       </c>
       <c r="D103" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E103" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -3109,10 +3231,10 @@
         <v>103</v>
       </c>
       <c r="D104" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E104" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -3120,10 +3242,10 @@
         <v>104</v>
       </c>
       <c r="D105" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E105" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -3131,10 +3253,10 @@
         <v>105</v>
       </c>
       <c r="D106" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E106" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -3142,10 +3264,10 @@
         <v>106</v>
       </c>
       <c r="D107" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E107" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -3153,10 +3275,10 @@
         <v>107</v>
       </c>
       <c r="D108" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E108" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -3164,10 +3286,10 @@
         <v>108</v>
       </c>
       <c r="D109" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E109" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -3175,10 +3297,10 @@
         <v>109</v>
       </c>
       <c r="D110" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E110" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -3186,10 +3308,10 @@
         <v>110</v>
       </c>
       <c r="D111" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E111" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -3197,10 +3319,10 @@
         <v>111</v>
       </c>
       <c r="D112" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E112" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -3208,10 +3330,10 @@
         <v>112</v>
       </c>
       <c r="D113" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E113" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -3219,10 +3341,10 @@
         <v>113</v>
       </c>
       <c r="D114" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E114" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -3230,10 +3352,10 @@
         <v>114</v>
       </c>
       <c r="D115" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E115" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -3241,10 +3363,10 @@
         <v>115</v>
       </c>
       <c r="D116" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E116" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -3252,10 +3374,10 @@
         <v>116</v>
       </c>
       <c r="D117" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E117" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -3263,10 +3385,10 @@
         <v>117</v>
       </c>
       <c r="D118" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E118" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -3274,10 +3396,10 @@
         <v>118</v>
       </c>
       <c r="D119" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E119" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -3285,10 +3407,10 @@
         <v>119</v>
       </c>
       <c r="D120" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E120" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -3296,10 +3418,10 @@
         <v>120</v>
       </c>
       <c r="D121" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E121" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -3307,10 +3429,10 @@
         <v>121</v>
       </c>
       <c r="D122" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E122" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -3318,10 +3440,10 @@
         <v>122</v>
       </c>
       <c r="D123" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E123" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -3329,10 +3451,10 @@
         <v>123</v>
       </c>
       <c r="D124" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E124" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -3340,10 +3462,10 @@
         <v>124</v>
       </c>
       <c r="D125" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E125" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -3351,10 +3473,10 @@
         <v>125</v>
       </c>
       <c r="D126" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E126" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -3362,10 +3484,10 @@
         <v>126</v>
       </c>
       <c r="D127" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E127" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -3373,10 +3495,10 @@
         <v>127</v>
       </c>
       <c r="D128" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E128" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -3384,10 +3506,10 @@
         <v>128</v>
       </c>
       <c r="D129" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E129" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -3395,10 +3517,10 @@
         <v>129</v>
       </c>
       <c r="D130" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E130" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -3406,10 +3528,10 @@
         <v>130</v>
       </c>
       <c r="D131" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E131" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -3417,10 +3539,10 @@
         <v>131</v>
       </c>
       <c r="D132" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E132" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -3428,10 +3550,10 @@
         <v>132</v>
       </c>
       <c r="D133" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E133" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -3439,10 +3561,10 @@
         <v>133</v>
       </c>
       <c r="D134" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E134" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -3450,10 +3572,10 @@
         <v>134</v>
       </c>
       <c r="D135" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E135" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -3461,10 +3583,10 @@
         <v>135</v>
       </c>
       <c r="D136" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E136" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -3472,10 +3594,10 @@
         <v>136</v>
       </c>
       <c r="D137" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E137" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -3483,10 +3605,10 @@
         <v>137</v>
       </c>
       <c r="D138" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E138" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -3494,10 +3616,10 @@
         <v>138</v>
       </c>
       <c r="D139" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E139" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -3505,10 +3627,10 @@
         <v>139</v>
       </c>
       <c r="D140" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E140" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -3516,10 +3638,10 @@
         <v>140</v>
       </c>
       <c r="D141" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E141" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -3527,10 +3649,10 @@
         <v>141</v>
       </c>
       <c r="D142" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E142" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -3538,10 +3660,10 @@
         <v>142</v>
       </c>
       <c r="D143" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E143" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -3549,10 +3671,10 @@
         <v>143</v>
       </c>
       <c r="D144" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E144" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -3560,10 +3682,10 @@
         <v>144</v>
       </c>
       <c r="D145" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E145" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -3571,10 +3693,10 @@
         <v>145</v>
       </c>
       <c r="D146" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E146" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -3582,10 +3704,10 @@
         <v>146</v>
       </c>
       <c r="D147" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E147" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -3593,10 +3715,10 @@
         <v>147</v>
       </c>
       <c r="D148" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E148" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -3604,10 +3726,10 @@
         <v>148</v>
       </c>
       <c r="D149" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E149" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -3615,10 +3737,10 @@
         <v>149</v>
       </c>
       <c r="D150" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E150" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -3626,10 +3748,10 @@
         <v>150</v>
       </c>
       <c r="D151" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E151" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -3637,10 +3759,10 @@
         <v>151</v>
       </c>
       <c r="D152" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E152" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -3648,10 +3770,10 @@
         <v>152</v>
       </c>
       <c r="D153" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E153" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -3659,10 +3781,10 @@
         <v>153</v>
       </c>
       <c r="D154" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E154" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -3670,10 +3792,10 @@
         <v>154</v>
       </c>
       <c r="D155" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E155" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -3681,10 +3803,10 @@
         <v>155</v>
       </c>
       <c r="D156" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E156" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -3692,10 +3814,10 @@
         <v>156</v>
       </c>
       <c r="D157" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E157" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -3703,10 +3825,10 @@
         <v>157</v>
       </c>
       <c r="D158" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E158" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -3714,10 +3836,10 @@
         <v>158</v>
       </c>
       <c r="D159" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E159" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -3725,10 +3847,10 @@
         <v>159</v>
       </c>
       <c r="D160" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E160" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -3736,10 +3858,10 @@
         <v>160</v>
       </c>
       <c r="D161" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E161" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -3747,10 +3869,10 @@
         <v>161</v>
       </c>
       <c r="D162" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E162" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -3758,10 +3880,10 @@
         <v>162</v>
       </c>
       <c r="D163" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E163" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -3769,10 +3891,10 @@
         <v>163</v>
       </c>
       <c r="D164" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E164" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -3780,10 +3902,10 @@
         <v>164</v>
       </c>
       <c r="D165" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E165" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -3791,10 +3913,10 @@
         <v>165</v>
       </c>
       <c r="D166" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E166" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -3802,10 +3924,10 @@
         <v>166</v>
       </c>
       <c r="D167" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E167" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -3813,10 +3935,10 @@
         <v>167</v>
       </c>
       <c r="D168" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E168" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -3824,10 +3946,10 @@
         <v>168</v>
       </c>
       <c r="D169" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E169" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -3835,10 +3957,10 @@
         <v>169</v>
       </c>
       <c r="D170" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E170" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -3846,10 +3968,10 @@
         <v>170</v>
       </c>
       <c r="D171" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E171" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -3857,10 +3979,10 @@
         <v>171</v>
       </c>
       <c r="D172" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E172" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -3868,10 +3990,10 @@
         <v>172</v>
       </c>
       <c r="D173" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E173" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -3879,10 +4001,10 @@
         <v>173</v>
       </c>
       <c r="D174" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E174" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -3890,10 +4012,10 @@
         <v>174</v>
       </c>
       <c r="D175" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E175" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -3901,10 +4023,10 @@
         <v>175</v>
       </c>
       <c r="D176" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E176" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -3912,10 +4034,10 @@
         <v>176</v>
       </c>
       <c r="D177" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E177" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -3923,10 +4045,10 @@
         <v>177</v>
       </c>
       <c r="D178" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E178" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -3934,10 +4056,10 @@
         <v>178</v>
       </c>
       <c r="D179" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E179" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -3945,10 +4067,10 @@
         <v>179</v>
       </c>
       <c r="D180" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E180" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -3956,10 +4078,10 @@
         <v>180</v>
       </c>
       <c r="D181" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E181" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -3967,10 +4089,10 @@
         <v>181</v>
       </c>
       <c r="D182" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E182" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
@@ -3978,10 +4100,10 @@
         <v>182</v>
       </c>
       <c r="D183" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E183" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -3989,10 +4111,10 @@
         <v>183</v>
       </c>
       <c r="D184" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E184" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -4000,10 +4122,10 @@
         <v>184</v>
       </c>
       <c r="D185" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E185" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
@@ -4011,10 +4133,10 @@
         <v>185</v>
       </c>
       <c r="D186" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E186" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
@@ -4022,10 +4144,10 @@
         <v>186</v>
       </c>
       <c r="D187" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E187" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -4033,10 +4155,10 @@
         <v>187</v>
       </c>
       <c r="D188" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E188" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
@@ -4044,10 +4166,10 @@
         <v>188</v>
       </c>
       <c r="D189" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E189" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -4055,10 +4177,10 @@
         <v>189</v>
       </c>
       <c r="D190" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E190" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -4066,10 +4188,10 @@
         <v>190</v>
       </c>
       <c r="D191" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E191" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -4077,10 +4199,10 @@
         <v>191</v>
       </c>
       <c r="D192" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E192" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -4088,10 +4210,10 @@
         <v>192</v>
       </c>
       <c r="D193" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E193" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -4099,10 +4221,10 @@
         <v>193</v>
       </c>
       <c r="D194" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E194" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -4110,10 +4232,10 @@
         <v>194</v>
       </c>
       <c r="D195" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E195" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -4121,10 +4243,10 @@
         <v>195</v>
       </c>
       <c r="D196" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E196" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -4132,10 +4254,10 @@
         <v>196</v>
       </c>
       <c r="D197" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E197" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
@@ -4143,10 +4265,10 @@
         <v>197</v>
       </c>
       <c r="D198" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E198" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -4154,10 +4276,10 @@
         <v>198</v>
       </c>
       <c r="D199" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E199" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -4165,10 +4287,10 @@
         <v>199</v>
       </c>
       <c r="D200" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E200" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
@@ -4176,10 +4298,10 @@
         <v>200</v>
       </c>
       <c r="D201" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E201" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
@@ -4187,10 +4309,10 @@
         <v>201</v>
       </c>
       <c r="D202" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E202" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
@@ -4198,10 +4320,10 @@
         <v>202</v>
       </c>
       <c r="D203" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E203" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -4209,10 +4331,10 @@
         <v>203</v>
       </c>
       <c r="D204" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E204" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -4220,10 +4342,10 @@
         <v>204</v>
       </c>
       <c r="D205" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E205" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
@@ -4231,10 +4353,10 @@
         <v>205</v>
       </c>
       <c r="D206" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E206" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
@@ -4242,10 +4364,10 @@
         <v>206</v>
       </c>
       <c r="D207" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E207" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
@@ -4253,10 +4375,10 @@
         <v>207</v>
       </c>
       <c r="D208" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E208" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
@@ -4264,10 +4386,10 @@
         <v>208</v>
       </c>
       <c r="D209" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E209" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
@@ -4275,10 +4397,10 @@
         <v>209</v>
       </c>
       <c r="D210" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E210" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
@@ -4286,10 +4408,10 @@
         <v>210</v>
       </c>
       <c r="D211" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E211" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
@@ -4297,10 +4419,10 @@
         <v>211</v>
       </c>
       <c r="D212" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E212" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
@@ -4308,10 +4430,10 @@
         <v>212</v>
       </c>
       <c r="D213" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E213" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
@@ -4319,10 +4441,10 @@
         <v>213</v>
       </c>
       <c r="D214" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E214" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
@@ -4330,10 +4452,10 @@
         <v>214</v>
       </c>
       <c r="D215" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E215" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
@@ -4341,10 +4463,10 @@
         <v>215</v>
       </c>
       <c r="D216" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E216" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
@@ -4352,10 +4474,10 @@
         <v>216</v>
       </c>
       <c r="D217" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E217" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
@@ -4363,10 +4485,10 @@
         <v>217</v>
       </c>
       <c r="D218" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E218" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
@@ -4374,10 +4496,10 @@
         <v>218</v>
       </c>
       <c r="D219" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E219" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
@@ -4385,10 +4507,10 @@
         <v>219</v>
       </c>
       <c r="D220" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E220" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
@@ -4396,10 +4518,10 @@
         <v>220</v>
       </c>
       <c r="D221" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E221" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
@@ -4407,10 +4529,10 @@
         <v>221</v>
       </c>
       <c r="D222" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E222" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
@@ -4418,10 +4540,10 @@
         <v>222</v>
       </c>
       <c r="D223" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E223" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
@@ -4429,10 +4551,10 @@
         <v>223</v>
       </c>
       <c r="D224" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E224" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
@@ -4440,10 +4562,10 @@
         <v>224</v>
       </c>
       <c r="D225" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E225" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
@@ -4451,10 +4573,10 @@
         <v>225</v>
       </c>
       <c r="D226" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E226" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
@@ -4462,10 +4584,10 @@
         <v>226</v>
       </c>
       <c r="D227" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E227" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
@@ -4473,10 +4595,10 @@
         <v>227</v>
       </c>
       <c r="D228" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E228" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
@@ -4484,10 +4606,10 @@
         <v>228</v>
       </c>
       <c r="D229" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E229" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
@@ -4495,10 +4617,10 @@
         <v>229</v>
       </c>
       <c r="D230" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E230" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
@@ -4506,10 +4628,10 @@
         <v>230</v>
       </c>
       <c r="D231" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E231" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
@@ -4517,10 +4639,10 @@
         <v>231</v>
       </c>
       <c r="D232" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E232" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
@@ -4528,10 +4650,10 @@
         <v>232</v>
       </c>
       <c r="D233" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E233" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
@@ -4539,10 +4661,10 @@
         <v>233</v>
       </c>
       <c r="D234" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E234" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
@@ -4550,10 +4672,10 @@
         <v>234</v>
       </c>
       <c r="D235" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E235" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
@@ -4561,10 +4683,10 @@
         <v>235</v>
       </c>
       <c r="D236" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E236" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
@@ -4572,10 +4694,10 @@
         <v>236</v>
       </c>
       <c r="D237" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E237" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
@@ -4583,10 +4705,10 @@
         <v>237</v>
       </c>
       <c r="D238" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E238" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
@@ -4594,10 +4716,10 @@
         <v>238</v>
       </c>
       <c r="D239" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E239" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
@@ -4605,10 +4727,10 @@
         <v>239</v>
       </c>
       <c r="D240" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E240" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
@@ -4616,10 +4738,10 @@
         <v>240</v>
       </c>
       <c r="D241" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E241" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
@@ -4627,10 +4749,10 @@
         <v>241</v>
       </c>
       <c r="D242" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E242" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
@@ -4638,10 +4760,10 @@
         <v>242</v>
       </c>
       <c r="D243" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E243" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
@@ -4649,10 +4771,10 @@
         <v>243</v>
       </c>
       <c r="D244" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E244" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
@@ -4660,10 +4782,10 @@
         <v>244</v>
       </c>
       <c r="D245" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E245" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
@@ -4671,10 +4793,10 @@
         <v>245</v>
       </c>
       <c r="D246" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E246" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
@@ -4682,10 +4804,10 @@
         <v>246</v>
       </c>
       <c r="D247" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E247" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
@@ -4693,10 +4815,10 @@
         <v>247</v>
       </c>
       <c r="D248" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E248" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
@@ -4704,10 +4826,10 @@
         <v>248</v>
       </c>
       <c r="D249" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E249" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
@@ -4715,10 +4837,10 @@
         <v>249</v>
       </c>
       <c r="D250" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E250" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
@@ -4726,10 +4848,10 @@
         <v>250</v>
       </c>
       <c r="D251" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E251" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
@@ -4737,10 +4859,10 @@
         <v>251</v>
       </c>
       <c r="D252" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E252" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
@@ -4748,10 +4870,10 @@
         <v>252</v>
       </c>
       <c r="D253" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E253" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
@@ -4759,10 +4881,10 @@
         <v>253</v>
       </c>
       <c r="D254" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E254" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
@@ -4770,10 +4892,10 @@
         <v>254</v>
       </c>
       <c r="D255" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E255" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
@@ -4781,10 +4903,10 @@
         <v>255</v>
       </c>
       <c r="D256" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E256" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
@@ -4792,10 +4914,10 @@
         <v>256</v>
       </c>
       <c r="D257" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E257" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
@@ -4803,10 +4925,10 @@
         <v>257</v>
       </c>
       <c r="D258" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E258" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
@@ -4814,10 +4936,10 @@
         <v>258</v>
       </c>
       <c r="D259" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E259" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
@@ -4825,10 +4947,10 @@
         <v>259</v>
       </c>
       <c r="D260" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E260" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
@@ -4836,10 +4958,10 @@
         <v>260</v>
       </c>
       <c r="D261" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E261" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
@@ -4847,10 +4969,10 @@
         <v>261</v>
       </c>
       <c r="D262" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E262" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
@@ -4858,10 +4980,10 @@
         <v>262</v>
       </c>
       <c r="D263" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E263" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
@@ -4869,10 +4991,10 @@
         <v>263</v>
       </c>
       <c r="D264" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E264" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
@@ -4880,10 +5002,10 @@
         <v>264</v>
       </c>
       <c r="D265" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E265" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
@@ -4891,10 +5013,10 @@
         <v>265</v>
       </c>
       <c r="D266" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E266" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
@@ -4902,10 +5024,10 @@
         <v>266</v>
       </c>
       <c r="D267" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E267" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
@@ -4913,10 +5035,10 @@
         <v>267</v>
       </c>
       <c r="D268" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E268" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
@@ -4924,10 +5046,10 @@
         <v>268</v>
       </c>
       <c r="D269" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E269" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
@@ -4935,10 +5057,10 @@
         <v>269</v>
       </c>
       <c r="D270" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E270" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
@@ -4946,10 +5068,10 @@
         <v>270</v>
       </c>
       <c r="D271" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E271" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
@@ -4957,10 +5079,10 @@
         <v>271</v>
       </c>
       <c r="D272" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E272" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.2">
@@ -4968,10 +5090,10 @@
         <v>272</v>
       </c>
       <c r="D273" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E273" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="377" spans="2:3" x14ac:dyDescent="0.2">
@@ -5005,14 +5127,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -5020,51 +5142,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="D2" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
       <c r="D3" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="D4" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="D5" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5072,7 +5194,7 @@
         <v>233</v>
       </c>
       <c r="D6" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -5080,39 +5202,39 @@
         <v>243</v>
       </c>
       <c r="D7" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="D8" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="D9" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="D10" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="D11" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -5125,7 +5247,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5140,13 +5262,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>281</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -5171,7 +5293,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5181,30 +5303,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>321</v>
       </c>
       <c r="B1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C1" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="D1" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
       <c r="B2" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>